<commit_message>
TN. RES values updated.
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee9/ieee9_2035.xlsx
+++ b/data/IEEE9/ieee9/ieee9_2035.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33E713C-E146-49C6-A2D5-CD90DA15C29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB54A3E7-8579-4A46-B420-413837444DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="722" firstSheet="23" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="17640" tabRatio="722" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13004,8 +13004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2238F2AC-228D-47B8-8C84-211710BC16D7}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27071,7 +27071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6451C0BC-1134-43AA-AB38-9EE91B1398E3}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:Y3"/>
     </sheetView>
   </sheetViews>

</xml_diff>